<commit_message>
changed the input files
</commit_message>
<xml_diff>
--- a/data/input/Auswertung Fahrplan 2025.xlsx
+++ b/data/input/Auswertung Fahrplan 2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kay\Documents\VCD\VCD Deutschlandtakt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD196183-0760-4D4A-88E5-DEAEAB7B6550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5CA4A6-F387-49B6-BDFC-97F02CE70557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FECA46D9-D90D-4033-9951-38453CE95731}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
   <si>
     <t>Verbindung nach</t>
   </si>
@@ -71,9 +71,6 @@
     <t>s_PKW [km]</t>
   </si>
   <si>
-    <t>Hannover Hbf (S2)</t>
-  </si>
-  <si>
     <t>Nienburg (RE)</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Hameln</t>
+  </si>
+  <si>
+    <t>Weetzen (S)</t>
   </si>
 </sst>
 </file>
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77DAD51C-77FA-4FD7-8AB1-4951DCBD21F1}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,19 +524,19 @@
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="D3">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="E3">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -582,48 +582,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>34</v>
       </c>
       <c r="D6">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E6">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>102</v>
-      </c>
-      <c r="C7">
-        <v>47</v>
-      </c>
-      <c r="D7">
-        <v>98</v>
-      </c>
-      <c r="E7">
-        <v>46</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -682,7 +662,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -762,7 +742,7 @@
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>60</v>
@@ -877,7 +857,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>76</v>
@@ -972,7 +952,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>86</v>
@@ -1012,7 +992,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -1107,7 +1087,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>32</v>
@@ -1127,7 +1107,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>23</v>
@@ -1222,7 +1202,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -1242,7 +1222,7 @@
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>22</v>
@@ -1282,7 +1262,7 @@
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -1337,7 +1317,7 @@
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1354,7 +1334,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>89</v>
@@ -1374,7 +1354,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>46</v>
@@ -1394,7 +1374,7 @@
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -1414,7 +1394,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1489,7 +1469,7 @@
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -1509,7 +1489,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -1564,7 +1544,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>16</v>

</xml_diff>